<commit_message>
refacter preparing data into function
</commit_message>
<xml_diff>
--- a/result_ERROR.xlsx
+++ b/result_ERROR.xlsx
@@ -27,7 +27,7 @@
     <numFmt numFmtId="166" formatCode="###0;###0"/>
     <numFmt numFmtId="167" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="39">
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -260,6 +260,11 @@
       <b val="1"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="4">
@@ -282,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -317,6 +322,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -326,7 +411,7 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -623,6 +708,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1868,16 +1958,48 @@
       <c r="B20" s="20" t="n"/>
     </row>
     <row r="21" ht="27.75" customHeight="1">
-      <c r="A21" s="20" t="n"/>
-      <c r="B21" s="20" t="n"/>
+      <c r="A21" s="112" t="inlineStr">
+        <is>
+          <t>it good</t>
+        </is>
+      </c>
+      <c r="B21" s="112" t="inlineStr">
+        <is>
+          <t>P.O. Nº</t>
+        </is>
+      </c>
+      <c r="C21" s="112" t="inlineStr">
+        <is>
+          <t>ITEM Nº</t>
+        </is>
+      </c>
+      <c r="D21" s="112" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="E21" s="113" t="n"/>
+      <c r="F21" s="112" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="27.75" customHeight="1">
-      <c r="A22" s="21" t="n"/>
-      <c r="B22" s="21" t="n"/>
-      <c r="C22" s="22" t="n"/>
-      <c r="D22" s="22" t="n"/>
-      <c r="E22" s="22" t="n"/>
-      <c r="F22" s="22" t="n"/>
+      <c r="A22" s="114" t="n"/>
+      <c r="B22" s="114" t="n"/>
+      <c r="C22" s="114" t="n"/>
+      <c r="D22" s="112" t="inlineStr">
+        <is>
+          <t>PCS</t>
+        </is>
+      </c>
+      <c r="E22" s="112" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="F22" s="114" t="n"/>
       <c r="G22" s="18" t="n"/>
       <c r="L22" s="49" t="n"/>
       <c r="M22" s="50" t="n"/>
@@ -2101,18 +2223,23 @@
     <row r="51" ht="17.25" customHeight="1"/>
     <row r="63" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="16">
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="B24:C24"/>
+    <mergeCell ref="F21:F22"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A4:G4"/>
+    <mergeCell ref="C21:C22"/>
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="A5:G5"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <conditionalFormatting sqref="J23:J35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>

</xml_diff>

<commit_message>
fix the packing list breaking line and now merge static before footer now working fine
</commit_message>
<xml_diff>
--- a/result_ERROR.xlsx
+++ b/result_ERROR.xlsx
@@ -1960,7 +1960,7 @@
     <row r="21" ht="27.75" customHeight="1">
       <c r="A21" s="112" t="inlineStr">
         <is>
-          <t>it good</t>
+          <t>NO.</t>
         </is>
       </c>
       <c r="B21" s="112" t="inlineStr">
@@ -1975,13 +1975,23 @@
       </c>
       <c r="D21" s="112" t="inlineStr">
         <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E21" s="112" t="inlineStr">
+        <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="E21" s="113" t="n"/>
-      <c r="F21" s="112" t="inlineStr">
-        <is>
-          <t>Description</t>
+      <c r="F21" s="113" t="n"/>
+      <c r="G21" s="112" t="inlineStr">
+        <is>
+          <t>Unit price (USD)</t>
+        </is>
+      </c>
+      <c r="H21" s="112" t="inlineStr">
+        <is>
+          <t>Amount (USD)</t>
         </is>
       </c>
     </row>
@@ -1989,18 +1999,19 @@
       <c r="A22" s="114" t="n"/>
       <c r="B22" s="114" t="n"/>
       <c r="C22" s="114" t="n"/>
-      <c r="D22" s="112" t="inlineStr">
+      <c r="D22" s="114" t="n"/>
+      <c r="E22" s="112" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="E22" s="112" t="inlineStr">
+      <c r="F22" s="112" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="F22" s="114" t="n"/>
-      <c r="G22" s="18" t="n"/>
+      <c r="G22" s="114" t="n"/>
+      <c r="H22" s="114" t="n"/>
       <c r="L22" s="49" t="n"/>
       <c r="M22" s="50" t="n"/>
       <c r="N22" s="51" t="n"/>
@@ -2223,11 +2234,11 @@
     <row r="51" ht="17.25" customHeight="1"/>
     <row r="63" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="F21:F22"/>
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A3:G3"/>
@@ -2236,10 +2247,12 @@
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="A26:G26"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="A5:G5"/>
-    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <conditionalFormatting sqref="J23:J35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>

</xml_diff>